<commit_message>
fix some gaming bug
</commit_message>
<xml_diff>
--- a/Assets/Excels/InstructionPack.xlsx
+++ b/Assets/Excels/InstructionPack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Project\GalFrameworkTest\Assets\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C54B1A-4D7D-438C-84D6-7C1501446F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19346B36-C88E-4D47-8D5C-5C38945E3A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>按序排列即可</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,6 +120,10 @@
   </si>
   <si>
     <t>final_part1_log5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>final_part1_log1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -448,7 +452,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -522,6 +526,9 @@
       <c r="B5" t="s">
         <v>15</v>
       </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">

</xml_diff>